<commit_message>
Added missing BOM excels
</commit_message>
<xml_diff>
--- a/m50,m40,m60 Pnp/Rev 1.0/BOM-speeduino v0.4.3 compatible PCB for m50nv rev1.0.xlsx
+++ b/m50,m40,m60 Pnp/Rev 1.0/BOM-speeduino v0.4.3 compatible PCB for m50nv rev1.0.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kemppain\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{49256836-EFCA-4DDA-A333-F871103BDCB9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B8759A-9340-446D-8527-4D03178AA85E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16515" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1100,31 +1105,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Note! The </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Green</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ones are optional components if hall crank sensor is used, instead of stock vr-sensor</t>
-    </r>
-  </si>
-  <si>
     <t>Speeduino vr-conditioner</t>
   </si>
   <si>
@@ -1263,6 +1243,31 @@
   </si>
   <si>
     <t>ULN2003A 1</t>
+  </si>
+  <si>
+    <r>
+      <t>Note! The</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Green</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ones are only installed if hall crank sensor is used, instead of stock vr-sensor(s). In that case the vr-conditioner is not installed at all.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1648,14 +1653,14 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2054,8 +2059,8 @@
   </sheetPr>
   <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="113" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="113" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2858,7 +2863,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>74</v>
@@ -2937,7 +2942,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>180</v>
@@ -3091,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>108</v>
@@ -3673,7 +3678,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D24" s="22" t="s">
         <v>107</v>
@@ -3832,16 +3837,16 @@
         <v>6</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D26" s="22" t="s">
         <v>107</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>229</v>
@@ -3857,13 +3862,13 @@
         <v>138</v>
       </c>
       <c r="L26" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="M26" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="N26" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="M26" s="30" t="s">
-        <v>296</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="O26" s="6">
         <v>0.25</v>
@@ -4410,7 +4415,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>71</v>
@@ -4643,7 +4648,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D37" s="22" t="s">
         <v>110</v>
@@ -4830,19 +4835,19 @@
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>61</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>300</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>301</v>
       </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3">
@@ -4855,13 +4860,13 @@
         <v>138</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="M40" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="M40" s="34" t="s">
+        <v>301</v>
+      </c>
+      <c r="N40" s="2" t="s">
         <v>302</v>
-      </c>
-      <c r="N40" s="2" t="s">
-        <v>303</v>
       </c>
       <c r="O40" s="5">
         <v>0.59</v>
@@ -4877,19 +4882,19 @@
       </c>
       <c r="S40" s="4"/>
       <c r="T40" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="U40" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="V40" t="s">
         <v>304</v>
       </c>
-      <c r="U40" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="V40" t="s">
+      <c r="W40" t="s">
         <v>305</v>
       </c>
-      <c r="W40" t="s">
+      <c r="X40" t="s">
         <v>306</v>
-      </c>
-      <c r="X40" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:24" ht="26.25" thickBot="1">
@@ -5273,14 +5278,14 @@
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>104</v>
@@ -5462,10 +5467,10 @@
       <c r="I50" s="8"/>
       <c r="J50" s="4"/>
       <c r="K50" s="8"/>
-      <c r="L50" s="34" t="s">
+      <c r="L50" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="M50" s="35"/>
+      <c r="M50" s="36"/>
       <c r="N50" s="32"/>
       <c r="O50" s="1" t="s">
         <v>68</v>
@@ -5490,12 +5495,12 @@
     </row>
     <row r="55" spans="1:24">
       <c r="C55" t="s">
-        <v>281</v>
+        <v>307</v>
       </c>
     </row>
     <row r="56" spans="1:24">
       <c r="C56" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>